<commit_message>
teste de integração e funcional
</commit_message>
<xml_diff>
--- a/invalidos-para-preencher.xlsx
+++ b/invalidos-para-preencher.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Nome Completo</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Funcional</t>
   </si>
   <si>
-    <t>Pedro Souza</t>
-  </si>
-  <si>
     <t>pedro.souza@email.com</t>
   </si>
   <si>
@@ -98,18 +95,6 @@
     <t>joao.santos@email</t>
   </si>
   <si>
-    <t>(11) 9123456</t>
-  </si>
-  <si>
-    <t>(21) 98765432199</t>
-  </si>
-  <si>
-    <t>() 999991111</t>
-  </si>
-  <si>
-    <t>(41) 87654abcd</t>
-  </si>
-  <si>
     <t>abc.def.789-00</t>
   </si>
   <si>
@@ -122,22 +107,43 @@
     <t>)!@.{[?.987-00</t>
   </si>
   <si>
-    <t>(11) 912345678</t>
-  </si>
-  <si>
-    <t>(21) 987654321</t>
-  </si>
-  <si>
-    <t>(31) 999991111</t>
-  </si>
-  <si>
-    <t>(41) 876543210</t>
-  </si>
-  <si>
     <t>pedro.souza@z</t>
   </si>
   <si>
     <t>último Souza</t>
+  </si>
+  <si>
+    <t>Pedro Souza2</t>
+  </si>
+  <si>
+    <t>Maria Oliveira%</t>
+  </si>
+  <si>
+    <t>(11)91234-56</t>
+  </si>
+  <si>
+    <t>(21)98765-432199</t>
+  </si>
+  <si>
+    <t>()99999-1111</t>
+  </si>
+  <si>
+    <t>(41)87654-abcd</t>
+  </si>
+  <si>
+    <t>(11)91234-5678</t>
+  </si>
+  <si>
+    <t>(21)98765-4321</t>
+  </si>
+  <si>
+    <t>(31)99999-1111</t>
+  </si>
+  <si>
+    <t>(41)87654-3210</t>
+  </si>
+  <si>
+    <t>321.654.987-@#</t>
   </si>
 </sst>
 </file>
@@ -185,8 +191,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -194,7 +200,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -490,7 +496,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +504,7 @@
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -513,7 +519,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -528,16 +534,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="2">
-        <v>32122000</v>
+        <v>31</v>
+      </c>
+      <c r="D2" s="3">
+        <v>36891</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -548,16 +554,16 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2">
-        <v>32212101</v>
+        <v>32</v>
+      </c>
+      <c r="D3" s="3">
+        <v>244</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -565,19 +571,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2985</v>
+      </c>
+      <c r="E4" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" s="3">
-        <v>35036000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -585,22 +591,22 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="3">
-        <v>40121995</v>
-      </c>
-      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2">
+        <v>35037</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -611,10 +617,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="3">
-        <v>15051990</v>
+        <v>35</v>
+      </c>
+      <c r="D6" s="2">
+        <v>33008</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -631,10 +637,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="3">
-        <v>20091985</v>
+        <v>36</v>
+      </c>
+      <c r="D7" s="2">
+        <v>31310</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -651,10 +657,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="3">
-        <v>28021995</v>
+        <v>37</v>
+      </c>
+      <c r="D8" s="2">
+        <v>34758</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -665,22 +671,22 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2">
+        <v>36717</v>
+      </c>
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="3">
-        <v>10071988</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -689,11 +695,12 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="E5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>